<commit_message>
adding a capacity limit to investments during initialization
</commit_message>
<xml_diff>
--- a/data/traderes/TradeRES_D2_1_Scenario_data_Corrected.xlsx
+++ b/data/traderes/TradeRES_D2_1_Scenario_data_Corrected.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\traderes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E67949-3751-4926-AE1F-349DB50D1C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9684C0E5-3C6F-4BDA-8B36-6E79119BFE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15840" tabRatio="921" firstSheet="2" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="28110" windowHeight="16440" tabRatio="921" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="3" r:id="rId1"/>
@@ -11789,11 +11789,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AM104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M22" sqref="M22"/>
+      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -25222,11 +25222,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:BI138"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <pane xSplit="6" ySplit="2" topLeftCell="BF3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R136" sqref="A1:R136"/>
+      <selection pane="bottomRight" activeCell="BQ142" sqref="BQ142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -25558,7 +25558,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:61" ht="28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>609</v>
       </c>
@@ -25701,7 +25701,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:61" ht="28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>609</v>
       </c>
@@ -25844,7 +25844,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:61" ht="28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>609</v>
       </c>
@@ -25987,7 +25987,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:61" ht="28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>610</v>
       </c>
@@ -26130,7 +26130,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="7" spans="1:61" ht="28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>610</v>
       </c>
@@ -26273,7 +26273,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="1:61" ht="28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>610</v>
       </c>
@@ -26416,7 +26416,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:61" ht="28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>178</v>
       </c>
@@ -26554,7 +26554,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:61" ht="28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>178</v>
       </c>
@@ -26692,7 +26692,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:61" ht="28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>184</v>
       </c>
@@ -26830,7 +26830,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="12" spans="1:61" ht="28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>184</v>
       </c>
@@ -26968,7 +26968,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="13" spans="1:61" ht="28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>611</v>
       </c>
@@ -27108,7 +27108,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="14" spans="1:61" ht="28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>611</v>
       </c>
@@ -27248,7 +27248,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="15" spans="1:61" ht="28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>611</v>
       </c>
@@ -27388,7 +27388,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="16" spans="1:61" ht="42" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:61" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>195</v>
       </c>
@@ -27456,7 +27456,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="17" spans="1:61" ht="42" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:61" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>195</v>
       </c>
@@ -27524,7 +27524,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="18" spans="1:61" ht="42" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>195</v>
       </c>
@@ -27592,7 +27592,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="19" spans="1:61" ht="42" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>203</v>
       </c>
@@ -27660,7 +27660,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="20" spans="1:61" ht="42" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>203</v>
       </c>
@@ -27728,7 +27728,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="21" spans="1:61" ht="42" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>203</v>
       </c>
@@ -27796,7 +27796,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" spans="1:61" ht="42" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>207</v>
       </c>
@@ -27865,7 +27865,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="23" spans="1:61" ht="42" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>211</v>
       </c>
@@ -27934,7 +27934,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="24" spans="1:61" ht="42" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>213</v>
       </c>
@@ -28003,7 +28003,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="25" spans="1:61" ht="28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>215</v>
       </c>
@@ -28071,7 +28071,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:61" ht="42" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>207</v>
       </c>
@@ -28140,7 +28140,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="27" spans="1:61" ht="42" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="69" t="s">
         <v>211</v>
       </c>
@@ -28211,7 +28211,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="28" spans="1:61" ht="42" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>213</v>
       </c>
@@ -28280,7 +28280,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="29" spans="1:61" ht="28" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>215</v>
       </c>
@@ -28348,7 +28348,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="30" spans="1:61" ht="42" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>207</v>
       </c>
@@ -28417,7 +28417,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="31" spans="1:61" ht="42" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>211</v>
       </c>
@@ -28486,7 +28486,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="32" spans="1:61" ht="42" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>213</v>
       </c>
@@ -28555,7 +28555,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="33" spans="1:61" ht="28" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>215</v>
       </c>
@@ -28626,7 +28626,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="34" spans="1:61" ht="28" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>218</v>
       </c>
@@ -28699,7 +28699,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="35" spans="1:61" ht="28" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>218</v>
       </c>
@@ -28771,7 +28771,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="36" spans="1:61" ht="28" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>221</v>
       </c>
@@ -28873,7 +28873,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="37" spans="1:61" ht="28" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>221</v>
       </c>
@@ -28975,7 +28975,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="38" spans="1:61" ht="28" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>224</v>
       </c>
@@ -29073,7 +29073,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="39" spans="1:61" s="62" customFormat="1" ht="28" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:61" s="62" customFormat="1" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="61" t="s">
         <v>224</v>
       </c>
@@ -29171,7 +29171,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="40" spans="1:61" ht="28" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:61" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>82</v>
       </c>
@@ -29260,7 +29260,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="41" spans="1:61" s="33" customFormat="1" ht="42" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:61" s="33" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="31" t="s">
         <v>229</v>
       </c>
@@ -29282,7 +29282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:61" s="33" customFormat="1" ht="42" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:61" s="33" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="31" t="s">
         <v>229</v>
       </c>
@@ -31969,7 +31969,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="76" spans="1:58" ht="42" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>285</v>
       </c>
@@ -32067,7 +32067,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="77" spans="1:58" ht="42" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>285</v>
       </c>
@@ -32229,7 +32229,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="80" spans="1:58" ht="42" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>288</v>
       </c>
@@ -32326,7 +32326,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="81" spans="1:58" ht="42" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>288</v>
       </c>
@@ -32499,7 +32499,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="84" spans="1:58" ht="42" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:58" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>291</v>
       </c>
@@ -32625,7 +32625,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="86" spans="1:58" s="65" customFormat="1" ht="28" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:58" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="64" t="s">
         <v>293</v>
       </c>
@@ -32753,7 +32753,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="87" spans="1:58" ht="28" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>293</v>
       </c>
@@ -32940,7 +32940,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="89" spans="1:58" ht="28" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>293</v>
       </c>
@@ -33047,7 +33047,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="90" spans="1:58" ht="28" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>293</v>
       </c>
@@ -33228,7 +33228,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="92" spans="1:58" ht="28" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>293</v>
       </c>
@@ -33335,7 +33335,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="93" spans="1:58" ht="28" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>293</v>
       </c>
@@ -34655,7 +34655,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="111" spans="1:42" ht="28" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:42" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="71" t="s">
         <v>315</v>
       </c>
@@ -34871,7 +34871,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="116" spans="1:44" ht="28" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:44" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="71" t="s">
         <v>325</v>
       </c>
@@ -35095,7 +35095,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="119" spans="1:44" ht="28" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:44" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="71" t="s">
         <v>325</v>
       </c>
@@ -36008,7 +36008,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="132" spans="1:23" ht="28" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>345</v>
       </c>
@@ -36261,7 +36261,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="136" spans="1:23" ht="28" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>353</v>
       </c>
@@ -36455,6 +36455,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:BI138" xr:uid="{00000000-0001-0000-0500-000000000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Storage"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="2">
       <filters>
         <filter val="electricity"/>
@@ -37081,15 +37086,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100577F9741E05B564FB56462B6304E09DC" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8dae23664d5be85499aa81160ae0fa0b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2be9f748-766b-46f3-b477-b73214dbaefe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6998ab8f9d1a82cbe3e44632c2589ab3" ns2:_="">
     <xsd:import namespace="2be9f748-766b-46f3-b477-b73214dbaefe"/>
@@ -37235,6 +37231,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33403C9F-F7D8-4D9C-ABE9-5CDDE161B5F6}">
   <ds:schemaRefs>
@@ -37252,14 +37257,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39B86DC8-3E2D-43CE-AD36-E688A1669DE3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C955985-112F-4095-965E-4E727DFEB72B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -37275,4 +37272,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39B86DC8-3E2D-43CE-AD36-E688A1669DE3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>